<commit_message>
- update columns' header - created pattern_test_set_creator.py - fixed one_to_many extraction in stat_viewer_new.py
</commit_message>
<xml_diff>
--- a/data/FB15k-237/implication_stats_train.xlsx
+++ b/data/FB15k-237/implication_stats_train.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shayansh/Documents/Workspace/Python/KGE_Pattern/data/FB15k-237/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FAD937-AE99-9141-A91A-41FCA3B9984E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B2037A-8A79-5641-9937-DA82997AE49A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="17480" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="17480" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t>/award/award_nominee/award_nominations./award/award_nomination/award_nominee</t>
   </si>
@@ -502,7 +502,10 @@
     <t>/people/ethnicity/geographic_distribution</t>
   </si>
   <si>
-    <t>Number of occurances per implication relation in the train set</t>
+    <t>relation</t>
+  </si>
+  <si>
+    <t>count</t>
   </si>
 </sst>
 </file>
@@ -906,14 +909,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>